<commit_message>
Updated notes to include getting related data from a DbContext object.
</commit_message>
<xml_diff>
--- a/Labs/Lab06/Lab6Rubric_CS295N.xlsx
+++ b/Labs/Lab06/Lab6Rubric_CS295N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS295N-CourseMaterials/Labs/Lab06/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F358445A-25BF-E641-8267-3BB2C39CEC07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3265C26E-DCAD-DE49-98A6-1EBEF65A32AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36240" yWindow="9160" windowWidth="14260" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36240" yWindow="9160" windowWidth="14260" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab3Rubric_CS295N" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
-    <t>-----------------------------------</t>
-  </si>
-  <si>
     <t>Actual</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>Code review by lab partner</t>
+  </si>
+  <si>
+    <t>Conterollers: debugging, action methods, and return types</t>
   </si>
 </sst>
 </file>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1004,38 +1004,38 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1090,12 +1090,12 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3">
         <f>SUM(B7:B15)</f>
@@ -1145,12 +1145,12 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>12</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3">
         <f>SUM(B19:B20)</f>
@@ -1190,12 +1190,12 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="3">
         <f>SUM(B24:B25)</f>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" s="10">
         <f>SUM(B16,B21, B26)</f>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FE8FBD-3C9C-F84F-8CF1-73E172DCB999}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C28"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1335,38 +1335,38 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1421,12 +1421,12 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3">
         <f>SUM(B7:B15)</f>
@@ -1476,12 +1476,12 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>12</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3">
         <f>SUM(B19:B20)</f>
@@ -1521,12 +1521,12 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="3">
         <f>SUM(B24:B25)</f>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" s="10">
         <f>SUM(B16,B21, B26)</f>

</xml_diff>

<commit_message>
Started a course outline, added links page, updated rubrics
</commit_message>
<xml_diff>
--- a/Labs/Lab06/Lab6Rubric_CS295N.xlsx
+++ b/Labs/Lab06/Lab6Rubric_CS295N.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS295N-CourseMaterials/Labs/Lab06/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/Labs/Lab06/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3265C26E-DCAD-DE49-98A6-1EBEF65A32AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3523C88A-6070-AE4C-92D8-A85978F47E8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36240" yWindow="9160" windowWidth="14260" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14260" windowHeight="14720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab3Rubric_CS295N" sheetId="1" r:id="rId1"/>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FE8FBD-3C9C-F84F-8CF1-73E172DCB999}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1543,7 +1543,7 @@
         <v>2</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="C26" s="3">
         <f>SUM(C24:C25)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C28" s="10">
         <f>SUM(C16,C21, C26)</f>
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added to the rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab06/Lab6Rubric_CS295N.xlsx
+++ b/Labs/Lab06/Lab6Rubric_CS295N.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/Labs/Lab06/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Repos\CS295N-CourseMaterials\Labs\Lab06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB30AD68-48A5-2546-89E9-BD066D1C4AD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0902853-806B-4ACF-877C-8160E64B82C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23520" windowHeight="14740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41556" yWindow="-1188" windowWidth="11136" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab3Rubric_CS295N" sheetId="1" r:id="rId1"/>
     <sheet name="Student Points" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="34">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -99,6 +110,30 @@
   </si>
   <si>
     <t>Database works on Azure</t>
+  </si>
+  <si>
+    <t>A page showing all messages</t>
+  </si>
+  <si>
+    <t>A page showing all stories</t>
+  </si>
+  <si>
+    <t>A page showing all comments</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>Comment is stored</t>
+  </si>
+  <si>
+    <t>Can't check</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>Good start.</t>
   </si>
 </sst>
 </file>
@@ -1018,12 +1053,12 @@
       <selection activeCell="F11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="44.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1057,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18">
+    <row r="7" spans="1:6" ht="17.399999999999999">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1555,18 +1590,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C8BAC4-7C35-B64C-9C0F-AC9B3324E891}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="44.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +1635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18">
+    <row r="7" spans="1:6" ht="17.399999999999999">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1648,447 +1683,492 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="B13" s="13">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="3">
-        <f>SUM(B11:B14)</f>
+      <c r="B16" s="3">
+        <f>SUM(B11:B15)</f>
         <v>35</v>
       </c>
-      <c r="C15" s="3">
-        <f>SUM(C11:C14)</f>
+      <c r="C16" s="3">
+        <f>SUM(C11:C15)</f>
         <v>35</v>
       </c>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="F16" s="6"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>3</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>3</v>
       </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="6" t="s">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>2</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="3">
-        <f>SUM(B18:B19)</f>
-        <v>5</v>
-      </c>
-      <c r="C20" s="3">
-        <f>SUM(C18:C19)</f>
-        <v>5</v>
-      </c>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1"/>
+      <c r="B21" s="3">
+        <f>SUM(B19:B20)</f>
+        <v>5</v>
+      </c>
+      <c r="C21" s="3">
+        <f>SUM(C19:C20)</f>
+        <v>5</v>
+      </c>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="1"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="10">
-        <f>SUM(B7,B15,B20)</f>
+      <c r="B23" s="10">
+        <f>SUM(B7,B16,B21)</f>
         <v>50</v>
       </c>
-      <c r="C22" s="10">
-        <f>SUM(C7,C15,C20)</f>
+      <c r="C23" s="10">
+        <f>SUM(C7,C16,C21)</f>
         <v>50</v>
       </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6">
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6">
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="4" t="s">
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="6" t="s">
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="4" t="s">
+      <c r="F27" s="6"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>2</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29">
-        <v>10</v>
-      </c>
-      <c r="C29">
-        <v>10</v>
-      </c>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="F30" s="6"/>
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="4" t="s">
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>9</v>
-      </c>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
         <v>23</v>
       </c>
-      <c r="B33">
-        <v>5</v>
-      </c>
-      <c r="C33">
-        <v>5</v>
-      </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="B34">
         <v>5</v>
       </c>
       <c r="C34">
         <v>5</v>
       </c>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="12" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B35">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C35">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="13">
+        <v>5</v>
+      </c>
+      <c r="C36" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B36">
-        <v>10</v>
-      </c>
-      <c r="C36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="7" t="s">
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="3">
-        <f>SUM(B33:B36)</f>
+      <c r="B39" s="3">
+        <f>SUM(B34:B38)</f>
         <v>35</v>
       </c>
-      <c r="C37" s="3">
-        <f>SUM(C33:C36)</f>
+      <c r="C39" s="3">
+        <f>SUM(C34:C38)</f>
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="8" t="s">
+    <row r="40" spans="1:6">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
         <v>7</v>
       </c>
-      <c r="B40">
+      <c r="B42">
         <v>3</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="6" t="s">
+    <row r="43" spans="1:6">
+      <c r="A43" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B41">
+      <c r="B43">
         <v>2</v>
       </c>
-      <c r="C41">
+      <c r="C43">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="2" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="3">
-        <f>SUM(B40:B41)</f>
-        <v>5</v>
-      </c>
-      <c r="C42" s="3">
-        <f>SUM(C40:C41)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="10">
-        <f>SUM(B29,B37,B42)</f>
-        <v>50</v>
-      </c>
-      <c r="C44" s="10">
-        <f>SUM(C29,C37,C42)</f>
-        <v>50</v>
+      <c r="B44" s="3">
+        <f>SUM(B42:B43)</f>
+        <v>5</v>
+      </c>
+      <c r="C44" s="3">
+        <f>SUM(C42:C43)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="A46" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="10">
+        <f>SUM(B30,B39,B44)</f>
+        <v>50</v>
+      </c>
+      <c r="C46" s="10">
+        <f>SUM(C30,C39,C44)</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:4">
+      <c r="A50" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>2</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51">
-        <v>10</v>
-      </c>
-      <c r="C51">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" s="4" customFormat="1">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="4" customFormat="1">
+      <c r="A55" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B53"/>
-      <c r="C53"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+      <c r="B55"/>
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
         <v>16</v>
       </c>
-      <c r="B55">
-        <v>5</v>
-      </c>
-      <c r="C55">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="12" t="s">
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B56">
-        <v>5</v>
-      </c>
-      <c r="C56">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="12" t="s">
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B57">
-        <v>15</v>
-      </c>
-      <c r="C57">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="12" t="s">
+      <c r="B60">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B58">
-        <v>10</v>
-      </c>
-      <c r="C58">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="7" t="s">
+      <c r="B61">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="3">
-        <f>SUM(B55:B58)</f>
+      <c r="B62" s="3">
+        <f>SUM(B57:B61)</f>
         <v>35</v>
       </c>
-      <c r="C59" s="3">
-        <f>SUM(C55:C58)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="8" t="s">
+      <c r="C62" s="3">
+        <f>SUM(C57:C61)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>7</v>
       </c>
-      <c r="B62">
+      <c r="B65">
         <v>3</v>
       </c>
-      <c r="C62">
+      <c r="C65">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="6" t="s">
+    <row r="66" spans="1:3">
+      <c r="A66" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B63">
+      <c r="B66">
         <v>2</v>
       </c>
-      <c r="C63">
+      <c r="C66">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="2" t="s">
+    <row r="67" spans="1:3">
+      <c r="A67" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="3">
-        <f>SUM(B62:B63)</f>
-        <v>5</v>
-      </c>
-      <c r="C64" s="3">
-        <f>SUM(C62:C63)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="9" t="s">
+      <c r="B67" s="3">
+        <f>SUM(B65:B66)</f>
+        <v>5</v>
+      </c>
+      <c r="C67" s="3">
+        <f>SUM(C65:C66)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="10">
-        <f>SUM(B51,B59,B64)</f>
+      <c r="B69" s="10">
+        <f>SUM(B53,B62,B67)</f>
         <v>50</v>
       </c>
-      <c r="C66" s="10">
-        <f>SUM(C51,C59,C64)</f>
-        <v>50</v>
+      <c r="C69" s="10">
+        <f>SUM(C53,C62,C67)</f>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>